<commit_message>
updates to 5/6 and 5/7
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-06.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-06.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu\Documents\Analysis\2016-04-12 RTDC Report since 03-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stu\Documents\GitHub\eaglep3-reporting\EC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Train Runs" sheetId="1" r:id="rId1"/>
@@ -2668,7 +2668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK165"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O100" sqref="O100"/>
     </sheetView>
   </sheetViews>
@@ -15661,8 +15661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>